<commit_message>
small updates regarding TFM_UPD tables for senssitivt of transport & investment
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslands_SensInvestment.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslands_SensInvestment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5CA347-413E-4850-897B-3188D8BBF8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1CA077-B2DE-4AC6-BBF5-02EC1AE92B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16332" yWindow="108" windowWidth="23412" windowHeight="15888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="456" windowWidth="23412" windowHeight="15888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>TimeSlice</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>LimType</t>
   </si>
   <si>
     <t>Attribute</t>
@@ -527,20 +521,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:M20"/>
+  <dimension ref="B3:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -548,20 +542,18 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -576,399 +568,393 @@
       <c r="I4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E5" t="s">
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="10" t="str">
+        <f>F5</f>
+        <v>*1.25</v>
+      </c>
+      <c r="G6" s="10" t="str">
+        <f t="shared" ref="G6:I6" si="0">G5</f>
+        <v>*1.25</v>
+      </c>
+      <c r="H6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="6" t="s">
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="10" t="str">
+        <f t="shared" ref="F7:F20" si="1">F6</f>
+        <v>*1.25</v>
+      </c>
+      <c r="G7" s="10" t="str">
+        <f t="shared" ref="G7:G20" si="2">G6</f>
+        <v>*1.25</v>
+      </c>
+      <c r="H7" s="10" t="str">
+        <f t="shared" ref="H7:H20" si="3">H6</f>
+        <v>*1.25</v>
+      </c>
+      <c r="I7" s="10" t="str">
+        <f t="shared" ref="I7:I20" si="4">I6</f>
+        <v>*1.25</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="10" t="str">
-        <f>H5</f>
-        <v>*1.25</v>
-      </c>
-      <c r="I6" s="10" t="str">
-        <f t="shared" ref="I6:K6" si="0">I5</f>
-        <v>*1.25</v>
-      </c>
-      <c r="J6" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K6" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L6" s="6" t="s">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G8" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H8" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I8" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="10" t="str">
-        <f t="shared" ref="H7:H20" si="1">H6</f>
-        <v>*1.25</v>
-      </c>
-      <c r="I7" s="10" t="str">
-        <f t="shared" ref="I7:I20" si="2">I6</f>
-        <v>*1.25</v>
-      </c>
-      <c r="J7" s="10" t="str">
-        <f t="shared" ref="J7:J20" si="3">J6</f>
-        <v>*1.25</v>
-      </c>
-      <c r="K7" s="10" t="str">
-        <f t="shared" ref="K7:K20" si="4">K6</f>
-        <v>*1.25</v>
-      </c>
-      <c r="L7" s="6" t="s">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G9" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H9" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I9" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I8" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J8" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K8" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L8" s="6" t="s">
+    <row r="10" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G10" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H10" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I10" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I9" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J9" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K9" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L9" s="6" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G11" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H11" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I11" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I10" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J10" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K10" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L10" s="6" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G12" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H12" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I12" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I11" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J11" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K11" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L11" s="7" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G13" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H13" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I13" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I12" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J12" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K12" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L12" s="8" t="s">
+    <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G14" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H14" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I14" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I13" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J13" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K13" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L13" s="8" t="s">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G15" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H15" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I15" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I14" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J14" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K14" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L14" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G16" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H16" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I16" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I15" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J15" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K15" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L15" s="7" t="s">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G17" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H17" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I17" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I16" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J16" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K16" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L16" t="s">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G18" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H18" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I18" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I17" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J17" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K17" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L17" s="9" t="s">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G19" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H19" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I19" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I18" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J18" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K18" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L18" s="9" t="s">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>*1.25</v>
+      </c>
+      <c r="G20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>*1.25</v>
+      </c>
+      <c r="H20" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>*1.25</v>
+      </c>
+      <c r="I20" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>*1.25</v>
+      </c>
+      <c r="J20" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I19" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J19" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K19" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>*1.25</v>
-      </c>
-      <c r="I20" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>*1.25</v>
-      </c>
-      <c r="J20" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>*1.25</v>
-      </c>
-      <c r="K20" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>*1.25</v>
-      </c>
-      <c r="L20" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>